<commit_message>
Created acceptance test plan spreadsheet
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunther\Desktop\Swen\team-project-2188-swen-261-01-b\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A34A9-AD70-41B7-AFB5-2FC2980DD2D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A3FEF4-F5D5-48E6-981C-D6D2F110A711}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t>Instructions</t>
   </si>
@@ -123,6 +123,123 @@
   </si>
   <si>
     <t xml:space="preserve">GK - 6/25/19.  </t>
+  </si>
+  <si>
+    <t>As a Player I want to play my turn so that I can move my pieces around the board.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given the Game is not over, When it is my turn, Then I should be able to move my pieces and play my turn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to resign because I know I'm going to lose. </t>
+  </si>
+  <si>
+    <t>Given that it is not my turn, when I click the resign button, then I will be taken back to the home page.</t>
+  </si>
+  <si>
+    <t>Given that it is not my turn, when my opponent clicks the resign button, then I will be notified of their resignation.</t>
+  </si>
+  <si>
+    <t>Given that it is my turn, when I click the resign button, then I will be taken back to the home page.</t>
+  </si>
+  <si>
+    <t>Given that it is my turn, when my opponent resigns and after I finish my turn, then I will be notified of their resignation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to sign out because I'm done playing. </t>
+  </si>
+  <si>
+    <t>Given the Game is not over When it in not my turn Then I must wait for my opponent to take their turn.</t>
+  </si>
+  <si>
+    <t>Given the Game is over When I choose to exit the Game Then I will be redirected to the lobby.</t>
+  </si>
+  <si>
+    <t>Given that it is my turn When I make a move Then the server should validate my move.</t>
+  </si>
+  <si>
+    <t>Given that my move is valid When I submit the move Then the server updates the Game with it.</t>
+  </si>
+  <si>
+    <t>Given that my move is valid When I choose to revert the move, Then I should be able to try another move.</t>
+  </si>
+  <si>
+    <t>Given that my move is not valid When the move is rejected Then I should be able to try another move.</t>
+  </si>
+  <si>
+    <t>Given I am in a game When I have not made a move Then I should have the option to resign.</t>
+  </si>
+  <si>
+    <t>Given that I want to resign When I click the resign button Then the Game will end.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am in a game When it is my turn Then I should have the option to move my pieces around the board. </t>
+  </si>
+  <si>
+    <t>Given that I am in a game When I am waiting for my opponent, Then I should have the option to resign.</t>
+  </si>
+  <si>
+    <t>Given two players are playing When one player hits the Resign button Then the game is over</t>
+  </si>
+  <si>
+    <t>Given a player is logged in When the sign out button is pressed Then the player is signed out</t>
+  </si>
+  <si>
+    <t>Given a player is signed out When the page refreshes Then the sign in option should be available again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to know when the game is over so that I can move on to other games. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to move my pieces so that I can win the game. </t>
+  </si>
+  <si>
+    <t>Given that it is my turn, When I drag a piece onto a valid square, Then I should be able to submit my turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to wait for my opponent to play their turn so that we have a fair match. </t>
+  </si>
+  <si>
+    <t>Given that it is not my turn When the page refreshes Then the application should check if it  is now my turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that there are no additional turns/moves possible, When the final Game board is displayed, Then I can see a message detailing how the game ended. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that the Game is over, When I see the final Game board, Then I should have a means to exit the game and return home. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I want to resign, When I click the resign button, Then the Game should stop and display the end game message. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to jump over my opponent's pieces so that I can win the game. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When I have multiple jump moves available, Then I can choose between them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to jump over multiple pieces so that I can crush my opponent's self-esteem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, when a multi-jump move is available, Then I must move my piece along that path. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to get king pieces so that I can move in any direction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given it is a Player's turn, When a piece reaches the king row, Then the piece should be promoted to a king. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When I drag a piece onto an invalid square, Then the piece should return to its original position and I should be shown an error message. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When one of my pieces is able to jump over an opponent piece, Then I am able to take that jump. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When multiple multi-jump paths are available, then I can choose which one I want to use. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a piece is a king, When the king piece is moving, Then the king piece has the option to go forward or backward. </t>
   </si>
 </sst>
 </file>
@@ -159,15 +276,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -184,11 +307,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -223,6 +355,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,11 +790,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H597"/>
+  <dimension ref="A1:I597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="C37" sqref="C37:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -866,164 +1010,335 @@
       <c r="E16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="17" spans="1:7" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="E22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C23" s="8"/>
       <c r="E23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C24" s="8"/>
       <c r="E24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C26" s="8"/>
       <c r="E26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="E27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="E28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" s="8"/>
       <c r="E29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C30" s="8"/>
       <c r="E30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C33" s="8"/>
       <c r="E33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="C34" s="8"/>
       <c r="E34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C35" s="8"/>
       <c r="E35" s="8"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="C36" s="8"/>
       <c r="E36" s="8"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
       <c r="G48" s="8"/>
@@ -3796,7 +4111,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Acceptance Test Plan spreadsheet.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunther\Desktop\Swen\team-project-2188-swen-261-01-b\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunther\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A34A9-AD70-41B7-AFB5-2FC2980DD2D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C0DD8-B7A1-4730-92F3-B3768BF098FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="86">
   <si>
     <t>Instructions</t>
   </si>
@@ -124,12 +124,177 @@
   <si>
     <t xml:space="preserve">GK - 6/25/19.  </t>
   </si>
+  <si>
+    <t>As a Player I want to play my turn so that I can move my pieces around the board.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given the Game is not over, When it is my turn, Then I should be able to move my pieces and play my turn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to resign because I know I'm going to lose. </t>
+  </si>
+  <si>
+    <t>Given that it is not my turn, when I click the resign button, then I will be taken back to the home page.</t>
+  </si>
+  <si>
+    <t>Given that it is not my turn, when my opponent clicks the resign button, then I will be notified of their resignation.</t>
+  </si>
+  <si>
+    <t>Given that it is my turn, when I click the resign button, then I will be taken back to the home page.</t>
+  </si>
+  <si>
+    <t>Given that it is my turn, when my opponent resigns and after I finish my turn, then I will be notified of their resignation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to sign out because I'm done playing. </t>
+  </si>
+  <si>
+    <t>Given the Game is not over When it in not my turn Then I must wait for my opponent to take their turn.</t>
+  </si>
+  <si>
+    <t>Given the Game is over When I choose to exit the Game Then I will be redirected to the lobby.</t>
+  </si>
+  <si>
+    <t>Given that it is my turn When I make a move Then the server should validate my move.</t>
+  </si>
+  <si>
+    <t>Given that my move is valid When I submit the move Then the server updates the Game with it.</t>
+  </si>
+  <si>
+    <t>Given that my move is valid When I choose to revert the move, Then I should be able to try another move.</t>
+  </si>
+  <si>
+    <t>Given that my move is not valid When the move is rejected Then I should be able to try another move.</t>
+  </si>
+  <si>
+    <t>Given I am in a game When I have not made a move Then I should have the option to resign.</t>
+  </si>
+  <si>
+    <t>Given that I want to resign When I click the resign button Then the Game will end.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am in a game When it is my turn Then I should have the option to move my pieces around the board. </t>
+  </si>
+  <si>
+    <t>Given that I am in a game When I am waiting for my opponent, Then I should have the option to resign.</t>
+  </si>
+  <si>
+    <t>Given two players are playing When one player hits the Resign button Then the game is over</t>
+  </si>
+  <si>
+    <t>Given a player is logged in When the sign out button is pressed Then the player is signed out</t>
+  </si>
+  <si>
+    <t>Given a player is signed out When the page refreshes Then the sign in option should be available again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to know when the game is over so that I can move on to other games. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to move my pieces so that I can win the game. </t>
+  </si>
+  <si>
+    <t>Given that it is my turn, When I drag a piece onto a valid square, Then I should be able to submit my turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to wait for my opponent to play their turn so that we have a fair match. </t>
+  </si>
+  <si>
+    <t>Given that it is not my turn When the page refreshes Then the application should check if it  is now my turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that there are no additional turns/moves possible, When the final Game board is displayed, Then I can see a message detailing how the game ended. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that the Game is over, When I see the final Game board, Then I should have a means to exit the game and return home. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I want to resign, When I click the resign button, Then the Game should stop and display the end game message. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to jump over my opponent's pieces so that I can win the game. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When I have multiple jump moves available, Then I can choose between them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to jump over multiple pieces so that I can crush my opponent's self-esteem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, when a multi-jump move is available, Then I must move my piece along that path. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Player I want to get king pieces so that I can move in any direction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given it is a Player's turn, When a piece reaches the king row, Then the piece should be promoted to a king. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When I drag a piece onto an invalid square, Then the piece should return to its original position and I should be shown an error message. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When one of my pieces is able to jump over an opponent piece, Then I am able to take that jump. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that it is my turn, When multiple multi-jump paths are available, then I can choose which one I want to use. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a piece is a king, When the king piece is moving, Then the king piece has the option to go forward or backward. </t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>IFB 7/18/19</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>No spaces  were accepted by the game</t>
+  </si>
+  <si>
+    <t>One player clicked resign, then the second player also clicked resign, but the first player had already resigned, so it broke</t>
+  </si>
+  <si>
+    <t>GDK 7/25/19</t>
+  </si>
+  <si>
+    <t>GDK 7/25/20</t>
+  </si>
+  <si>
+    <t>GDK 7/25/21</t>
+  </si>
+  <si>
+    <t>GDK 7/25/22</t>
+  </si>
+  <si>
+    <t>GDK 7/25/23</t>
+  </si>
+  <si>
+    <t>GDK 7/25/24</t>
+  </si>
+  <si>
+    <t>GDK 7/25/25</t>
+  </si>
+  <si>
+    <t>GDK 7/25/26</t>
+  </si>
+  <si>
+    <t>GDK 7/25/27</t>
+  </si>
+  <si>
+    <t>GDK 7/25/28</t>
+  </si>
+  <si>
+    <t>GDK 7/25/29</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,16 +323,41 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -184,11 +374,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -223,6 +437,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,11 +872,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H597"/>
+  <dimension ref="A1:I597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -703,7 +929,12 @@
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
@@ -715,7 +946,12 @@
       <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="62.7" x14ac:dyDescent="0.55000000000000004">
@@ -727,8 +963,18 @@
       <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="78.349999999999994" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7"/>
@@ -739,7 +985,12 @@
       <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="62.7" x14ac:dyDescent="0.55000000000000004">
@@ -751,7 +1002,12 @@
       <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
@@ -763,7 +1019,12 @@
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
@@ -775,7 +1036,12 @@
       <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="41" x14ac:dyDescent="0.4">
@@ -789,8 +1055,12 @@
       <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11"/>
     </row>
@@ -803,7 +1073,12 @@
       <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
@@ -815,7 +1090,12 @@
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="94" x14ac:dyDescent="0.55000000000000004">
@@ -827,7 +1107,12 @@
       <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
@@ -836,7 +1121,12 @@
         <v>11</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
@@ -845,7 +1135,12 @@
         <v>12</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="62.7" x14ac:dyDescent="0.55000000000000004">
@@ -854,7 +1149,12 @@
         <v>13</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
@@ -863,167 +1163,492 @@
         <v>14</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="17" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E32" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="C34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="C36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
       <c r="G48" s="8"/>
@@ -3774,6 +4399,7 @@
       <c r="G597" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C2:C597 E2:E597 G2:G597">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"Pass"</formula>
@@ -3796,7 +4422,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updates Acceptance Test Plan spreadsheet with Enhancement user stories.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunther\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunther\Desktop\Swen\team-project-2188-swen-261-01-b\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C0DD8-B7A1-4730-92F3-B3768BF098FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC27A26A-6436-409F-8449-45E7B6376254}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,14 @@
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="100">
   <si>
     <t>Instructions</t>
   </si>
@@ -288,6 +294,48 @@
   </si>
   <si>
     <t>GDK 7/25/29</t>
+  </si>
+  <si>
+    <t>As a Player I want to watch other games that are currently in progress so that I can improve my chekcers knowledge.</t>
+  </si>
+  <si>
+    <t>Given I am spectating a checkers game, When a new move is made by either player, Then I will see the move on my game view.</t>
+  </si>
+  <si>
+    <t>Given I am spectating a checkers game, When I click the Exit button, Then I will be redirected to back to the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a player I want to seave completed games so that I can replay them later and study my technique. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I just finished a checkers game, When I exit the game, Then the game will be saved to my account. </t>
+  </si>
+  <si>
+    <t>As a player I want to replay my completed checkers games so that I can improve my checkers skills.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I have completed a checkers game, When I am on the home page, then I should see a list of my previously completed checkers games. </t>
+  </si>
+  <si>
+    <t>Given that I am on the home page, When I click on a saved game to replay, Then I will be redirected to a game view of that games initial starting position.</t>
+  </si>
+  <si>
+    <t>Given that I am replaying a game, When I click the Next button, Then the next move from the game will be updated on the game view.</t>
+  </si>
+  <si>
+    <t>Given that I am replaying a game, When I click the Previous button, Then the previous move form the game will be reverted on the game view.</t>
+  </si>
+  <si>
+    <t>Given that I am replaying a game, When I click the exit button, I will return to the home page.</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given there is a checkers game in progress, When I click the spectate button, Then I should be redirected into a game view watching the current game. </t>
+  </si>
+  <si>
+    <t>GDK 8/1/19</t>
   </si>
 </sst>
 </file>
@@ -357,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -398,11 +446,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -447,14 +506,46 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -872,11 +963,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I597"/>
+  <dimension ref="A1:J597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -889,10 +980,12 @@
     <col min="6" max="6" width="60" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" customWidth="1"/>
     <col min="8" max="8" width="60" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.88671875" style="5"/>
+    <col min="9" max="9" width="10.88671875" style="5"/>
+    <col min="10" max="10" width="47.94140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="10.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -917,8 +1010,14 @@
       <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="31.35" x14ac:dyDescent="0.4">
+      <c r="I1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="31.35" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -936,8 +1035,9 @@
         <v>71</v>
       </c>
       <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -953,8 +1053,9 @@
         <v>71</v>
       </c>
       <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" ht="62.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="62.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>24</v>
@@ -975,8 +1076,9 @@
       <c r="H4" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="78.349999999999994" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="78.349999999999994" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -992,8 +1094,9 @@
         <v>71</v>
       </c>
       <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" ht="62.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="62.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>27</v>
@@ -1009,8 +1112,9 @@
         <v>71</v>
       </c>
       <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -1026,8 +1130,9 @@
         <v>71</v>
       </c>
       <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -1043,8 +1148,9 @@
         <v>71</v>
       </c>
       <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" ht="41" x14ac:dyDescent="0.4">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="41" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -1063,8 +1169,9 @@
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -1080,8 +1187,9 @@
         <v>71</v>
       </c>
       <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -1097,8 +1205,9 @@
         <v>71</v>
       </c>
       <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" ht="94" x14ac:dyDescent="0.55000000000000004">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="94" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>28</v>
@@ -1114,8 +1223,9 @@
         <v>71</v>
       </c>
       <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
@@ -1128,8 +1238,9 @@
         <v>71</v>
       </c>
       <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
@@ -1142,8 +1253,9 @@
         <v>71</v>
       </c>
       <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="62.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="62.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
@@ -1156,8 +1268,9 @@
         <v>71</v>
       </c>
       <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
@@ -1170,8 +1283,9 @@
         <v>71</v>
       </c>
       <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
@@ -1186,8 +1300,9 @@
         <v>71</v>
       </c>
       <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
@@ -1199,8 +1314,9 @@
         <v>71</v>
       </c>
       <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="2" t="s">
         <v>40</v>
       </c>
@@ -1212,8 +1328,9 @@
         <v>71</v>
       </c>
       <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
@@ -1225,8 +1342,9 @@
         <v>71</v>
       </c>
       <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
@@ -1238,8 +1356,9 @@
         <v>71</v>
       </c>
       <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
@@ -1251,8 +1370,9 @@
         <v>71</v>
       </c>
       <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1264,8 +1384,9 @@
         <v>71</v>
       </c>
       <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
@@ -1277,8 +1398,9 @@
         <v>71</v>
       </c>
       <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="13"/>
       <c r="B25" s="13" t="s">
         <v>46</v>
@@ -1291,8 +1413,9 @@
         <v>71</v>
       </c>
       <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>55</v>
       </c>
@@ -1307,8 +1430,9 @@
         <v>71</v>
       </c>
       <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="2" t="s">
         <v>56</v>
       </c>
@@ -1320,8 +1444,9 @@
         <v>71</v>
       </c>
       <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="2" t="s">
         <v>48</v>
       </c>
@@ -1333,8 +1458,9 @@
         <v>71</v>
       </c>
       <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="13"/>
       <c r="B29" s="13" t="s">
         <v>46</v>
@@ -1347,8 +1473,9 @@
         <v>71</v>
       </c>
       <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1363,8 +1490,9 @@
         <v>71</v>
       </c>
       <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1376,8 +1504,9 @@
         <v>71</v>
       </c>
       <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1394,8 +1523,9 @@
       <c r="H32" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1407,8 +1537,9 @@
         <v>71</v>
       </c>
       <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="13"/>
       <c r="B34" s="13" t="s">
         <v>37</v>
@@ -1421,8 +1552,9 @@
         <v>71</v>
       </c>
       <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
@@ -1437,8 +1569,9 @@
         <v>71</v>
       </c>
       <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
         <v>51</v>
@@ -1451,8 +1584,9 @@
         <v>71</v>
       </c>
       <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
@@ -1469,9 +1603,9 @@
       <c r="H37" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="I37" s="16"/>
-    </row>
-    <row r="38" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="2" t="s">
         <v>58</v>
       </c>
@@ -1485,9 +1619,9 @@
       <c r="H38" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="I38" s="16"/>
-    </row>
-    <row r="39" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
         <v>59</v>
@@ -1502,9 +1636,9 @@
       <c r="H39" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="I39" s="16"/>
-    </row>
-    <row r="40" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2" t="s">
         <v>53</v>
       </c>
@@ -1521,9 +1655,9 @@
       <c r="H40" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="I40" s="16"/>
-    </row>
-    <row r="41" spans="1:9" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" ht="47.35" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A41" s="13"/>
       <c r="B41" s="13" t="s">
         <v>66</v>
@@ -1538,9 +1672,9 @@
       <c r="H41" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="I41" s="16"/>
-    </row>
-    <row r="42" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
@@ -1557,9 +1691,9 @@
       <c r="H42" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I42" s="16"/>
-    </row>
-    <row r="43" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A43" s="13"/>
       <c r="B43" s="13" t="s">
         <v>61</v>
@@ -1574,9 +1708,9 @@
       <c r="H43" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I43" s="16"/>
-    </row>
-    <row r="44" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2" t="s">
         <v>62</v>
       </c>
@@ -1593,9 +1727,9 @@
       <c r="H44" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I44" s="16"/>
-    </row>
-    <row r="45" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A45" s="13"/>
       <c r="B45" s="13" t="s">
         <v>68</v>
@@ -1610,9 +1744,9 @@
       <c r="H45" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="I45" s="16"/>
-    </row>
-    <row r="46" spans="1:9" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
@@ -1629,9 +1763,9 @@
       <c r="H46" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="I46" s="16"/>
-    </row>
-    <row r="47" spans="1:9" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A47" s="13"/>
       <c r="B47" s="13" t="s">
         <v>69</v>
@@ -1646,89 +1780,189 @@
       <c r="H47" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="I47" s="16"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:10" ht="62.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
       <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I48" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C49" s="8"/>
       <c r="E49" s="8"/>
       <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I49" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="17" customFormat="1" ht="31.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="20" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A51" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="C52" s="8"/>
       <c r="E52" s="8"/>
       <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I52" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="C53" s="8"/>
       <c r="E53" s="8"/>
       <c r="G53" s="8"/>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I53" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C54" s="8"/>
       <c r="E54" s="8"/>
       <c r="G54" s="8"/>
-    </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I54" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="C55" s="8"/>
       <c r="E55" s="8"/>
       <c r="G55" s="8"/>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I55" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C56" s="8"/>
       <c r="E56" s="8"/>
       <c r="G56" s="8"/>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I56" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" s="8"/>
       <c r="E57" s="8"/>
       <c r="G57" s="8"/>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I57" s="8"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" s="8"/>
       <c r="E58" s="8"/>
       <c r="G58" s="8"/>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I58" s="8"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" s="8"/>
       <c r="E59" s="8"/>
       <c r="G59" s="8"/>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I59" s="8"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C60" s="8"/>
       <c r="E60" s="8"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C61" s="8"/>
       <c r="E61" s="8"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C62" s="8"/>
       <c r="E62" s="8"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C63" s="8"/>
       <c r="E63" s="8"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="8"/>
       <c r="E64" s="8"/>
       <c r="G64" s="8"/>
@@ -4401,23 +4635,31 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C2:C597 E2:E597 G2:G597">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D597 F2:F597 H2:H597">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="7" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="8" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I59">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E597 C2:C597 G2:G597" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E597 C2:C597 G2:G597 I2:I59" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>